<commit_message>
Updated .gitignore to exclude test-output files
</commit_message>
<xml_diff>
--- a/src/test/resources/config/TestData.xlsx
+++ b/src/test/resources/config/TestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bloss\src\RESTAssuredBDD\src\test\resources\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9534D7BB-7B10-48A7-B488-79315F59DCD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E57F09C3-1548-48E1-988A-8A5CE28DBC35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21870" yWindow="780" windowWidth="16515" windowHeight="9930" xr2:uid="{A4134BD0-6F01-40A1-AA77-D194A9223826}"/>
+    <workbookView xWindow="-19320" yWindow="2565" windowWidth="16020" windowHeight="8175" xr2:uid="{A4134BD0-6F01-40A1-AA77-D194A9223826}"/>
   </bookViews>
   <sheets>
     <sheet name="POST" sheetId="1" r:id="rId1"/>
@@ -507,7 +507,7 @@
   <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I8" sqref="I8"/>
+      <selection activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>